<commit_message>
imlemented Data Driven for RS creation campaign java file
</commit_message>
<xml_diff>
--- a/TC-RS.xlsx
+++ b/TC-RS.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CB81EC-FA57-4C98-891B-FE30D83ABF35}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EBE9B0-EB9A-47CD-8076-012CD7BDDB4C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="5895" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5895" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CampCreation" sheetId="1" r:id="rId1"/>
     <sheet name="Responses" sheetId="2" r:id="rId2"/>
     <sheet name="Reports" sheetId="3" r:id="rId3"/>
     <sheet name="CustActReport" sheetId="4" r:id="rId4"/>
-    <sheet name="LivePreview" sheetId="6" r:id="rId5"/>
+    <sheet name="LivePreview&amp;Delete" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -44,9 +44,6 @@
     <t>id:48167</t>
   </si>
   <si>
-    <t>Verify the Brand campaign scenarios</t>
-  </si>
-  <si>
     <t>Login to AC1</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>"Create New Campaigns" Page should display</t>
   </si>
   <si>
-    <t>"Brand Campaign" should be selected as Campaign type</t>
-  </si>
-  <si>
     <t>Select a Campaign language as "English" From the Dropdown list.</t>
   </si>
   <si>
@@ -86,12 +80,6 @@
     <t>"Existing campaign tool tip" should be display in English.</t>
   </si>
   <si>
-    <t>verify that "Brand" Text Field should display in campaign info section</t>
-  </si>
-  <si>
-    <t>"Brand" Text Field should display in Campaign info section and user able to enter "Campaign Name", "Brand Name", and "Description"</t>
-  </si>
-  <si>
     <t>Verify that user able to upload a Logo by clicking on "Choose" button and should able to enter the "Sender Name" in Text Box.</t>
   </si>
   <si>
@@ -128,9 +116,6 @@
     <t>Verify that "Cancel", "Save Draft", and "Create Campaign" buttons are enabled and Check user able to click on "Create campaign" button.</t>
   </si>
   <si>
-    <t>Click on "Live Preview" button of scheduled campaign.</t>
-  </si>
-  <si>
     <t>Click "Close Preview" button.</t>
   </si>
   <si>
@@ -141,12 +126,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Live Preview page "Feed Back" Section should display with proper data.</t>
-  </si>
-  <si>
-    <t>Live Preview page "Thank you" Section should display with proper data.</t>
   </si>
   <si>
     <t>id:54703</t>
@@ -302,34 +281,61 @@
     <t>Navigate to Campaigns Page : click campaigns under "Customer Feed Back" Tab</t>
   </si>
   <si>
+    <t>user should be able to enter the data in "Subject", "Intro-Banner", "Body Copy", and "Signature".</t>
+  </si>
+  <si>
+    <t>User should be able to verify the personalisation tool tip display in English Language.</t>
+  </si>
+  <si>
+    <t>Verify that User able to select a "Date and Time" from Scheduled section of Date picker and Time Dropdown button.</t>
+  </si>
+  <si>
+    <t>Verify that Created campaign displaying in "Scheduled campaign" section.</t>
+  </si>
+  <si>
+    <t>"Created campaign" should be display in "Scheduled campaign" section, "Edit", "Live Preview", and "Delete" buttons are enabled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Delete campaign" confirmation pop up should display. and </t>
+  </si>
+  <si>
+    <t>id:48066</t>
+  </si>
+  <si>
+    <t>Verify the location campaign scenarios</t>
+  </si>
+  <si>
+    <t>Select a Campaign type "Location" from the Dropdown list.</t>
+  </si>
+  <si>
+    <t>"Location" should be selected as Campaign type</t>
+  </si>
+  <si>
+    <t>verify that "Location" Text Field should display in campaign info section</t>
+  </si>
+  <si>
+    <t>"Location" Text Field should display in Campaign info section and user able to enter "Campaign Name" and "Description. And should able to select Location from auto suggesstion list.</t>
+  </si>
+  <si>
+    <t>Enter the Partial/Full location name in Location Text Field and able to select the location from Auto Suggesstion List.</t>
+  </si>
+  <si>
+    <t>User should able to Enter the Location name in "Location" Text Field and should able to select the Location From Auto Suggession List.</t>
+  </si>
+  <si>
+    <t>Verify the Brand campaign scenarios</t>
+  </si>
+  <si>
     <t>Select a Campaign type "Brand" from the Dropdown list.</t>
   </si>
   <si>
-    <t>user should be able to enter the data in "Subject", "Intro-Banner", "Body Copy", and "Signature".</t>
-  </si>
-  <si>
-    <t>User should be able to verify the personalisation tool tip display in English Language.</t>
-  </si>
-  <si>
-    <t>Verify that User able to select a "Date and Time" from Scheduled section of Date picker and Time Dropdown button.</t>
-  </si>
-  <si>
-    <t>Verify that Created campaign displaying in "Scheduled campaign" section.</t>
-  </si>
-  <si>
-    <t>"Created campaign" should be display in "Scheduled campaign" section, "Edit", "Live Preview", and "Delete" buttons are enabled.</t>
-  </si>
-  <si>
-    <t>"Live Preview" page should be display."Email View" should display with proper data.</t>
-  </si>
-  <si>
-    <t>click on "Give a Review button" of Live Preview page</t>
-  </si>
-  <si>
-    <t>Click on "Send Feed Back" button of scheduled campaign.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Delete campaign" confirmation pop up should display. and </t>
+    <t>"Brand Campaign" should be selected as Campaign type</t>
+  </si>
+  <si>
+    <t>verify that "Brand" Text Field should display in campaign info section</t>
+  </si>
+  <si>
+    <t>"Brand" Text Field should display in Campaign info section and user able to enter "Campaign Name", "Brand Name", and "Description"</t>
   </si>
 </sst>
 </file>
@@ -661,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -707,7 +713,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -716,7 +722,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -725,10 +731,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -736,10 +742,10 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -747,10 +753,10 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -758,10 +764,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -769,10 +775,10 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -780,36 +786,36 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -817,49 +823,49 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -867,36 +873,36 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -904,110 +910,259 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1052,80 +1207,80 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1170,80 +1325,80 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1288,85 +1443,85 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1376,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C087E27-36FA-4201-A2EF-223704CA841E}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,88 +1566,112 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
splitted the campaign creation classes
</commit_message>
<xml_diff>
--- a/TC-RS.xlsx
+++ b/TC-RS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DCB470-6A4E-44ED-8403-28B11C11BBAE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A35F0F-B243-458F-95B3-32388D79CF41}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="5895" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="5895" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CampCreation" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Click on Responses link of Searched Processed Campaign.</t>
-  </si>
-  <si>
-    <t>Responses page should be display and campaign name selected as default and Campaign "From Date" should be Campaign Scheduled date and "To Date" Should be Todays date.</t>
   </si>
   <si>
     <t>id:54704</t>
@@ -332,10 +329,19 @@
     <t>"Brand" Text Field should display in Campaign info section and user able to enter "Campaign Name", "Brand Name", and "Description"</t>
   </si>
   <si>
-    <t>Verify that the Data is displayed in Average Score, Overall Star Rating with Table data.  </t>
-  </si>
-  <si>
-    <t>All the reports should be displayed and should match with the UI Table data.</t>
+    <t>Verify that the Data is displayed in Average Score, Overall Star Rating section.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responses page should be display. </t>
+  </si>
+  <si>
+    <t>Campaign name selected as default and Campaign "From Date" should be Campaign Scheduled date and "To Date" Should be Todays date.</t>
+  </si>
+  <si>
+    <t>Verify that the Responses Page UI Table Data should match with Downloaded Table Data.</t>
+  </si>
+  <si>
+    <t>All the reports should be displayed and Downloaded Table data should match with the UI Table data.</t>
   </si>
 </sst>
 </file>
@@ -667,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -742,7 +748,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -764,10 +770,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -799,10 +805,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -815,7 +821,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -849,10 +855,10 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -865,7 +871,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -886,7 +892,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
@@ -923,32 +929,30 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>85</v>
-      </c>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
@@ -956,7 +960,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -965,32 +969,30 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -998,10 +1000,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1009,10 +1011,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="E29" s="1"/>
     </row>
@@ -1020,71 +1022,69 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>33</v>
@@ -1094,10 +1094,10 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>33</v>
@@ -1107,60 +1107,73 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1172,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EA1EB5-B96C-435B-AF55-228DB5DCC33C}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1252,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1250,37 +1263,45 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>69</v>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1325,10 +1346,10 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,40 +1386,40 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1443,10 +1464,10 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,45 +1504,45 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1566,10 +1587,10 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1600,54 +1621,54 @@
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1663,15 +1684,15 @@
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Classes Of RS
</commit_message>
<xml_diff>
--- a/TC-RS.xlsx
+++ b/TC-RS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BAC25D-17A8-4736-B4C8-55B194019871}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2066E6-75BC-4934-BB0E-50826D31D401}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14550" windowHeight="5895" tabRatio="726" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -379,6 +379,39 @@
   </si>
   <si>
     <t>"Location" Text Field should display in Campaign info section and user able to enter "Campaign Name", "Location Name", and "Description"</t>
+  </si>
+  <si>
+    <t>Verify the MLC campaign scenarios</t>
+  </si>
+  <si>
+    <t>id:54917</t>
+  </si>
+  <si>
+    <t>Select a Campaign type "MLC" from the Dropdown list.</t>
+  </si>
+  <si>
+    <t>"MLC" should be selected as Campaign type</t>
+  </si>
+  <si>
+    <t>verify that "Location" Text Field should display in campaign info section with Multi select Location List Box.</t>
+  </si>
+  <si>
+    <t>"MLC" Text Field should display with Multi Select list box in Campaign info section and user able to enter "Campaign Name" and "Description" in Campaign info section.</t>
+  </si>
+  <si>
+    <t>Verify that "Add", "Add All", "Remove", and "Remove All" Buttons tool tips.</t>
+  </si>
+  <si>
+    <t>"Add", "Add All", "Remove", and "Remove All" Buttons tool tips should display in Respective Languages.</t>
+  </si>
+  <si>
+    <t>sdssd</t>
+  </si>
+  <si>
+    <t>sfsf</t>
+  </si>
+  <si>
+    <t>fdf</t>
   </si>
 </sst>
 </file>
@@ -710,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,6 +1244,245 @@
         <v>81</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1591,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C087E27-36FA-4201-A2EF-223704CA841E}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,16 +1903,25 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1863,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9617CC-FEA7-4413-B6E7-804BCBCCAE12}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
classes separated according to Module wise
</commit_message>
<xml_diff>
--- a/TC-RS.xlsx
+++ b/TC-RS.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2066E6-75BC-4934-BB0E-50826D31D401}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0FCBC0-D796-4D60-8A80-5AA65FB1FA61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14550" windowHeight="5895" tabRatio="726" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14550" windowHeight="5895" tabRatio="726" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CampCreation" sheetId="1" r:id="rId1"/>
-    <sheet name="Responses" sheetId="2" r:id="rId2"/>
-    <sheet name="Reports" sheetId="3" r:id="rId3"/>
-    <sheet name="CustActReport" sheetId="4" r:id="rId4"/>
-    <sheet name="LivePreview&amp;Delete" sheetId="6" r:id="rId5"/>
-    <sheet name="DraftCamp" sheetId="7" r:id="rId6"/>
+    <sheet name="EditCamp" sheetId="9" r:id="rId2"/>
+    <sheet name="Responses" sheetId="2" r:id="rId3"/>
+    <sheet name="Reports" sheetId="3" r:id="rId4"/>
+    <sheet name="CustActReport" sheetId="4" r:id="rId5"/>
+    <sheet name="LivePreview&amp;Delete" sheetId="6" r:id="rId6"/>
+    <sheet name="DraftCamp" sheetId="7" r:id="rId7"/>
+    <sheet name="ProcessedCamp" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="191">
   <si>
     <t>ID</t>
   </si>
@@ -204,12 +206,6 @@
     <t>User able to download the CSV with the same details in the table </t>
   </si>
   <si>
-    <t>Check that there won't be any line breaks in the CSV for the added comments   </t>
-  </si>
-  <si>
-    <t>There shouldn't be any line breaks in the downloaded CSV  </t>
-  </si>
-  <si>
     <t>Click on Customer Activity Report link of Searched Processed Campaign.</t>
   </si>
   <si>
@@ -412,6 +408,220 @@
   </si>
   <si>
     <t>fdf</t>
+  </si>
+  <si>
+    <t>Check that Downloaded CSV data should match with the Customer activity Report's UI Table Data</t>
+  </si>
+  <si>
+    <t>Downloaded CSV data should match with the Customer activity Report's UI Table Data</t>
+  </si>
+  <si>
+    <t>id:54908</t>
+  </si>
+  <si>
+    <t>Verify the Location campaign scenarios - Customer Activity page</t>
+  </si>
+  <si>
+    <t>id:54930</t>
+  </si>
+  <si>
+    <t>Verify the MLC campaign scenarios - Customer Activity page</t>
+  </si>
+  <si>
+    <t>id:54205</t>
+  </si>
+  <si>
+    <t>Verify the Brand campaign scenarios - Update/Edit</t>
+  </si>
+  <si>
+    <t>Verify if Edit button is enabled when the campaign is scheduled </t>
+  </si>
+  <si>
+    <t>Edit button shall be displayed as enabled </t>
+  </si>
+  <si>
+    <t>Verify if Edit button is changed to Reschedule for failed campaigns  </t>
+  </si>
+  <si>
+    <t>Reschedule button is displayed for the failed   campaigns</t>
+  </si>
+  <si>
+    <t>Verify Update Campaign, Live Preview and Cancel button should be displayed when user clicks on Edit on scheduled campaign </t>
+  </si>
+  <si>
+    <t>Update campaign,"Live Preview" and "Cancel" button shall be displayed  </t>
+  </si>
+  <si>
+    <t>Verify if user is allowed to update all the fields </t>
+  </si>
+  <si>
+    <t>User shall be able to update all the fields.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to download Template </t>
+  </si>
+  <si>
+    <t>User shall be able to download the "Template"  </t>
+  </si>
+  <si>
+    <t>Verify if user is able to upload email using the template </t>
+  </si>
+  <si>
+    <t>User shall be able to upload email using the template</t>
+  </si>
+  <si>
+    <t>Verify personalization of tokens by entering the Body copy if tokens are getting replaced with First name and Last name in Live preview and Email Template Email Template replaced with First name and Last name in Live preview and Email Template  </t>
+  </si>
+  <si>
+    <t>1) Personalization of Tokens shall be replaced with the "First Name" and "Last name in Live preview
+2) Email Template shall be replaced with "First name" and "Last Last name" in Live preview and Email Template.  </t>
+  </si>
+  <si>
+    <t>Verify in the email template, if user updated a logo in update campaign then updated campaign should be displayed in Email Template </t>
+  </si>
+  <si>
+    <t>1) User shall be able to update the logo in updated campaign
+2) Updated campaign shall be displayed in "Email Template" </t>
+  </si>
+  <si>
+    <t>Searched Scheduled campaign's "Edit", "Live Preview" and "Delete" buttons should be enabled. If searched campaign is a failed campaign then "Edit" button should be replaced with "Reschedule" button.</t>
+  </si>
+  <si>
+    <t>Veify that Scheduled campaign's "Edit", "Live Preview" and "Delete" buttons are enabled. If searched campaign is a failed campaign then check the "Edit" button should replace with "Reschedule" button.</t>
+  </si>
+  <si>
+    <t>Click on "Edit/Reschedule(if failed camp)" button</t>
+  </si>
+  <si>
+    <t>Scheduled campaign should be display in editable mode.</t>
+  </si>
+  <si>
+    <t>Verify "Contact info" section displaying as we selcted "Brand" as campaign type and Contact info tool tip is display in respective language.</t>
+  </si>
+  <si>
+    <t>Verify that "Update Campaign" button is disabled when User not edited any field in "Edit Scheduled Campaign" page.</t>
+  </si>
+  <si>
+    <t>Update Campaign button should be disabled when User not edited any field in "Edit Scheduled Campaign" page.</t>
+  </si>
+  <si>
+    <t>Verify that User is able to upload the edited "Email Template"(By Replacing the Token values with older values) and Campaign Logo.</t>
+  </si>
+  <si>
+    <t>User should be able to Upload the Latest "Email Template" and Campaign Logo</t>
+  </si>
+  <si>
+    <t>Verify that User is able to change the campaign Schedule time</t>
+  </si>
+  <si>
+    <t>User should be able to change the campaign schedule time.</t>
+  </si>
+  <si>
+    <t>Verify that "Update Campaign" button is Enabled when User edited atleast 1 field in "Edit Scheduled Campaign" page.</t>
+  </si>
+  <si>
+    <t>"Update Campaign" button should be enabled.</t>
+  </si>
+  <si>
+    <t>Click on "Update Campaign" button</t>
+  </si>
+  <si>
+    <t>"Update Campaign" pop up should be display.</t>
+  </si>
+  <si>
+    <t>Click on "View all Campaigns" button in "Update Campaign" pop up</t>
+  </si>
+  <si>
+    <t>Page should be Redirect to Campaign's page</t>
+  </si>
+  <si>
+    <t>Click on "Live Preview" button of Edited Scheduled campaign</t>
+  </si>
+  <si>
+    <t>"Live Preview" page should be display.</t>
+  </si>
+  <si>
+    <t>Verify personalization of tokens of entered in the Subject, Banner, Body Copy and Thank you Fields if tokens are getting replaced with First name and Last name in Live preview.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personalization of Tokens shall be replaced with the "First Name" and "Last name in Live preview
+</t>
+  </si>
+  <si>
+    <t>id:54715</t>
+  </si>
+  <si>
+    <t>Verify the Location campaign scenarios - Update/Edit campaign</t>
+  </si>
+  <si>
+    <t>Pre-requisite: User should be logged into TransparenSee and should have access to Review Solicitation. @ACcount_Name</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Verify if Edit button is enabled when the campaign is scheduled  </t>
+  </si>
+  <si>
+    <t>Verify if Edit button is disabled with the Campaign is processing (Scheduled time)  </t>
+  </si>
+  <si>
+    <t>Edit button is displayed as "disabled"  </t>
+  </si>
+  <si>
+    <t>Verify if Edit button is changed to Reschedule for failed campaigns   </t>
+  </si>
+  <si>
+    <t>Verify if user is allowed to update all the fields including scheduled time </t>
+  </si>
+  <si>
+    <t>User shall be able to update all the fields including scheduled time</t>
+  </si>
+  <si>
+    <t>Verify if user is able to download Template  </t>
+  </si>
+  <si>
+    <t>User shall be able to download the "Template" </t>
+  </si>
+  <si>
+    <t>Verify if user is able to upload email using the template </t>
+  </si>
+  <si>
+    <t>User shall be able to upload email using the template </t>
+  </si>
+  <si>
+    <t>Verify personalization of tokens by entering the Body copy if tokens are getting replaced with First name and Last name in Live preview and Email Template replaced with First name and Last name in Live preview and Email Template  </t>
+  </si>
+  <si>
+    <t>1) Personalization of Tokens shall be replaced with the "First Name" and "Last name in Live preview2)Email Template shall be replaced with "First name" and "Last Last name" in Live preview and Email Template.</t>
+  </si>
+  <si>
+    <t>Verify if user added the logo during campaign creation same logo is getting displayed  </t>
+  </si>
+  <si>
+    <t>1)User shall be able to add the logo.
+2)Added logo shall be displayed. </t>
+  </si>
+  <si>
+    <t>Verify message highlighted in yellow is displayed when user clicks on "This campaign has been saved in Draft Mode.
+This campaign can be confirmed and scheduled by pressing the 'Create Campaign'
+button below"</t>
+  </si>
+  <si>
+    <t>Following message shall be displayed as in yellow color
+"This campaign has been saved in Draft Mode. This campaign can be confirmed and scheduled by pressing the 'Create Campaign' button below" </t>
+  </si>
+  <si>
+    <t>id:54923</t>
+  </si>
+  <si>
+    <t>Verify the MLC campaign scenarios - Update/Edit</t>
+  </si>
+  <si>
+    <t> Verify when user selects MLC campaign in Campaign Type Contact Info section and MLC name is getting displayed </t>
+  </si>
+  <si>
+    <t> MLC name shall be displayed </t>
   </si>
 </sst>
 </file>
@@ -745,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -818,7 +1028,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -840,10 +1050,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -875,10 +1085,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -891,7 +1101,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -925,10 +1135,10 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -941,15 +1151,15 @@
         <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>25</v>
@@ -962,7 +1172,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
@@ -999,10 +1209,10 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>33</v>
@@ -1017,10 +1227,10 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1059,7 +1269,7 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -1081,10 +1291,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E29" s="1"/>
     </row>
@@ -1116,10 +1326,10 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>33</v>
@@ -1129,10 +1339,10 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1143,7 +1353,7 @@
         <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -1177,10 +1387,10 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>33</v>
@@ -1193,7 +1403,7 @@
         <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E38" s="1"/>
     </row>
@@ -1201,7 +1411,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>26</v>
@@ -1238,10 +1448,10 @@
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>33</v>
@@ -1256,10 +1466,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1298,7 +1508,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -1320,10 +1530,10 @@
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1355,10 +1565,10 @@
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>33</v>
@@ -1368,10 +1578,10 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -1382,7 +1592,7 @@
         <v>18</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E55" s="1"/>
     </row>
@@ -1416,10 +1626,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>33</v>
@@ -1432,7 +1642,7 @@
         <v>23</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E59" s="1"/>
     </row>
@@ -1440,7 +1650,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>26</v>
@@ -1477,10 +1687,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>33</v>
@@ -1493,11 +1703,365 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9213576C-118C-42BE-8F2E-3C0F8E5CC6A9}">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="41" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EA1EB5-B96C-435B-AF55-228DB5DCC33C}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +2125,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1572,7 +2136,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1580,18 +2144,18 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1604,13 +2168,13 @@
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1618,12 +2182,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBC9AB6-1BAF-4631-BB8D-163F9EE683EF}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,7 +2259,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1706,7 +2270,7 @@
         <v>47</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1714,10 +2278,10 @@
         <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1728,7 +2292,7 @@
         <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1736,12 +2300,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3834F5-F8E4-432F-B054-DCFBDE612648}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,18 +2377,18 @@
         <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
@@ -1835,7 +2399,7 @@
         <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1848,10 +2412,176 @@
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>55</v>
+      <c r="D19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1859,12 +2589,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C087E27-36FA-4201-A2EF-223704CA841E}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,15 +2626,15 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1912,7 +2642,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1920,7 +2650,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1939,54 +2669,54 @@
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2002,29 +2732,29 @@
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
@@ -2055,54 +2785,54 @@
     </row>
     <row r="21" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="3:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
@@ -2118,21 +2848,21 @@
         <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9617CC-FEA7-4413-B6E7-804BCBCCAE12}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -2176,10 +2906,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2218,7 +2948,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -2240,10 +2970,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2275,10 +3005,10 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -2291,7 +3021,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -2325,10 +3055,10 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -2341,7 +3071,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -2362,7 +3092,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
@@ -2386,10 +3116,10 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>33</v>
@@ -2399,13 +3129,13 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2417,10 +3147,10 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2459,7 +3189,7 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -2481,10 +3211,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E29" s="1"/>
     </row>
@@ -2516,10 +3246,10 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>33</v>
@@ -2532,7 +3262,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -2566,10 +3296,10 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>33</v>
@@ -2582,7 +3312,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="1"/>
     </row>
@@ -2590,7 +3320,7 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>26</v>
@@ -2614,10 +3344,10 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>33</v>
@@ -2627,10 +3357,10 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>33</v>
@@ -2639,4 +3369,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F71ACB-000F-401B-BB58-60B4FC784606}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implemented listener, changed base class and other few changes
</commit_message>
<xml_diff>
--- a/TC-RS.xlsx
+++ b/TC-RS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820719BF-81E9-4405-8BAB-E6CD5F16C4DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9367EF-4251-4011-94EE-E00669D1EDAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="5895" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="5895" tabRatio="726" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CampCreation" sheetId="11" r:id="rId1"/>
@@ -14,8 +14,9 @@
     <sheet name="Reports" sheetId="3" r:id="rId4"/>
     <sheet name="CustActReport" sheetId="4" r:id="rId5"/>
     <sheet name="LivePreview&amp;Delete" sheetId="6" r:id="rId6"/>
-    <sheet name="DraftCamp" sheetId="7" r:id="rId7"/>
+    <sheet name="DraftBrand" sheetId="7" r:id="rId7"/>
     <sheet name="ProcessedCamp" sheetId="8" r:id="rId8"/>
+    <sheet name="DraftLoc" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -961,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6817DE79-FB62-4535-895E-FA5F05AC2BD3}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -2793,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9617CC-FEA7-4413-B6E7-804BCBCCAE12}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,234 +3058,6 @@
       </c>
       <c r="E21" s="1" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3304,4 +3077,265 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C82C7F-1130-4129-82A5-CBC538B5CC9D}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="63" customWidth="1"/>
+    <col min="4" max="4" width="59" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>